<commit_message>
Cleaned credentials - only Node-1 device, removed old configs.csv
</commit_message>
<xml_diff>
--- a/credentials_store.xlsx
+++ b/credentials_store.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="device_credentials" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -27,24 +27,17 @@
     </font>
     <font>
       <b val="1"/>
-      <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00366092"/>
-        <bgColor rgb="00366092"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -52,14 +45,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -426,32 +425,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="11" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="48" customWidth="1" min="4" max="4"/>
-    <col width="18" customWidth="1" min="5" max="5"/>
-    <col width="35" customWidth="1" min="6" max="6"/>
-    <col width="36" customWidth="1" min="7" max="7"/>
-    <col width="19" customWidth="1" min="8" max="8"/>
-    <col width="17" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
-    <col width="16" customWidth="1" min="11" max="11"/>
-    <col width="18" customWidth="1" min="12" max="12"/>
-    <col width="22" customWidth="1" min="13" max="13"/>
-    <col width="15" customWidth="1" min="14" max="14"/>
-    <col width="8" customWidth="1" min="15" max="15"/>
-    <col width="36" customWidth="1" min="16" max="16"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -538,32 +518,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PH-03</t>
+          <t>Node-1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>PumpHouse3</t>
+          <t>Node-1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NRPVCJ0ZX0J23U62</t>
+          <t>FOU6A6Z5UPM99P2W</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>8080932314:AAE3QYoTXbLbjKuCF-YqeBJK_BQVTxO7yG0</t>
+          <t>8162248845:AAGGtHV047WpFx5CMDsUxubvVU1Tm3DJrtI</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>879323820</t>
+          <t>8656817616</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1bK3vX9wYZcDefGhIjKlMnOpQrStUvWxY</t>
+          <t>1O-yz6vgWDGgD2XIIay5jUFHr1L9GKi_k</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -571,377 +551,33 @@
           <t>AKfycbzXYZ123ABC456DEF789GHI012JKL</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>0.6</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>100.0</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>300</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="N2" t="n">
+        <v>100</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Primary device - active deployment</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>PH-04</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>PumpHouse4</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>AWI3VOXT0WQ1AJVP</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>8080932314:AAE3QYoTXbLbjKuCF-YqeBJK_BQVTxO7yG0</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>879323820</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>1bK3vX9wYZcDefGhIjKlMnOpQrStUvWxY</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>AKfycbzXYZ123ABC456DEF789GHI012JKL</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>0.6</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>100.0</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>Secondary device - active</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>PR00-70</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Project70</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>9G2O6FOYECROP3WL</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>8080932314:AAE3QYoTXbLbjKuCF-YqeBJK_BQVTxO7yG0</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>879323820</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>1bK3vX9wYZcDefGhIjKlMnOpQrStUvWxY</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>AKfycbzXYZ123ABC456DEF789GHI012JKL</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>0.6</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>100.0</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>Telegram disabled - testing</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>KB04-72</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Himalaya1</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>XYZ789ABCDEFGHIJK</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>8080932314:AAE3QYoTXbLbjKuCF-YqeBJK_BQVTxO7yG0</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>879323820</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>1bK3vX9wYZcDefGhIjKlMnOpQrStUvWxY</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>AKfycbzXYZ123ABC456DEF789GHI012JKL</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>0.6</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>100.0</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>Mountain region deployment</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>TEST-01</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>TestDevice</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>TESTKEY123456789A</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>8080932314:AAE3QYoTXbLbjKuCF-YqeBJK_BQVTxO7yG0</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>879323820</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>1bK3vX9wYZcDefGhIjKlMnOpQrStUvWxY</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>AKfycbzXYZ123ABC456DEF789GHI012JKL</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>100.0</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>Inactive test device</t>
+          <t>New deployment - Node-1</t>
         </is>
       </c>
     </row>

</xml_diff>